<commit_message>
bug fix in table
</commit_message>
<xml_diff>
--- a/ListAllSamplesRNAseq_Discovery_2014.xlsx
+++ b/ListAllSamplesRNAseq_Discovery_2014.xlsx
@@ -751,7 +751,7 @@
     <t>Sample_US-1505888</t>
   </si>
   <si>
-    <t>Sample_US-1505988</t>
+    <t>Sample_US-1505998</t>
   </si>
   <si>
     <t>Sample_US-1505895</t>
@@ -1250,7 +1250,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1274,7 +1274,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="13" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1294,7 +1294,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1302,7 +1302,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1322,7 +1322,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1346,7 +1346,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1366,7 +1366,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1390,7 +1390,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1406,7 +1406,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1422,11 +1422,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1434,7 +1434,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="6" fillId="3" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1442,11 +1442,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1454,7 +1454,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1462,7 +1462,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1474,15 +1474,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1502,15 +1502,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1522,7 +1522,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1562,7 +1562,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1570,15 +1570,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1698,7 +1698,7 @@
   <dimension ref="A2:K112"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B89" activeCellId="1" sqref="A65:A88 B89"/>
+      <selection pane="topLeft" activeCell="B89" activeCellId="0" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3594,8 +3594,8 @@
   </sheetPr>
   <dimension ref="A1:H88"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A65" activeCellId="0" sqref="A65:A88"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5779,7 +5779,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A65:A88 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>